<commit_message>
Reestructuration for R workflow
</commit_message>
<xml_diff>
--- a/data/Datos_para_modelo/Datos_MP_BiomasaEst_Altura.xlsx
+++ b/data/Datos_para_modelo/Datos_MP_BiomasaEst_Altura.xlsx
@@ -510,7 +510,7 @@
         <v>39</v>
       </c>
       <c r="G2" t="n">
-        <v>5.281664473626443</v>
+        <v>4487.835088689853</v>
       </c>
       <c r="H2" t="n">
         <v>8.128549616571769</v>
@@ -544,7 +544,7 @@
         <v>124</v>
       </c>
       <c r="G3" t="n">
-        <v>6.433409435956624</v>
+        <v>25561.64806043415</v>
       </c>
       <c r="H3" t="n">
         <v>9.218264612091087</v>
@@ -580,7 +580,7 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>17.49383225642263</v>
+        <v>26798.32530343667</v>
       </c>
       <c r="H4" t="n">
         <v>6.722502663638702</v>
@@ -616,7 +616,7 @@
         </is>
       </c>
       <c r="G5" t="n">
-        <v>22.61329653493919</v>
+        <v>28009.14661183589</v>
       </c>
       <c r="H5" t="n">
         <v>6.285530827627425</v>
@@ -650,7 +650,7 @@
         <v>128</v>
       </c>
       <c r="G6" t="n">
-        <v>6.465086621876428</v>
+        <v>27742.41330128168</v>
       </c>
       <c r="H6" t="n">
         <v>5.159819164850667</v>
@@ -686,7 +686,7 @@
         </is>
       </c>
       <c r="G7" t="n">
-        <v>17.28202098231563</v>
+        <v>25257.48039457412</v>
       </c>
       <c r="H7" t="n">
         <v>5.680132462114407</v>
@@ -722,7 +722,7 @@
         </is>
       </c>
       <c r="G8" t="n">
-        <v>12.04245423558994</v>
+        <v>40861.41173042744</v>
       </c>
       <c r="H8" t="n">
         <v>8.419512052728908</v>
@@ -758,7 +758,7 @@
         </is>
       </c>
       <c r="G9" t="n">
-        <v>23.91554396330685</v>
+        <v>44488.16753834767</v>
       </c>
       <c r="H9" t="n">
         <v>8.965542866992999</v>
@@ -794,7 +794,7 @@
         </is>
       </c>
       <c r="G10" t="n">
-        <v>34.65837055795748</v>
+        <v>46536.72255404371</v>
       </c>
       <c r="H10" t="n">
         <v>8.689432706898923</v>
@@ -828,7 +828,7 @@
         <v>142</v>
       </c>
       <c r="G11" t="n">
-        <v>6.568664817800408</v>
+        <v>36947.75795729789</v>
       </c>
       <c r="H11" t="n">
         <v>7.896802142812189</v>
@@ -864,7 +864,7 @@
         </is>
       </c>
       <c r="G12" t="n">
-        <v>23.02404735753278</v>
+        <v>29493.56771244427</v>
       </c>
       <c r="H12" t="n">
         <v>8.419512052728908</v>
@@ -896,7 +896,7 @@
         <v>79</v>
       </c>
       <c r="G13" t="n">
-        <v>5.983878344500106</v>
+        <v>10176.31997172458</v>
       </c>
       <c r="H13" t="n">
         <v>10.58072611288203</v>
@@ -932,7 +932,7 @@
         </is>
       </c>
       <c r="G14" t="n">
-        <v>10.97600706779813</v>
+        <v>13664.97120493165</v>
       </c>
       <c r="H14" t="n">
         <v>12.38372703248685</v>
@@ -966,7 +966,7 @@
         </is>
       </c>
       <c r="G15" t="n">
-        <v>11.10531141531023</v>
+        <v>13663.22656188528</v>
       </c>
       <c r="H15" t="n">
         <v>10.15426611885745</v>
@@ -1000,7 +1000,7 @@
         <v>106</v>
       </c>
       <c r="G16" t="n">
-        <v>6.276955470745572</v>
+        <v>17684.37078971498</v>
       </c>
       <c r="H16" t="n">
         <v>10.91618590254367</v>
@@ -1034,7 +1034,7 @@
         <v>95</v>
       </c>
       <c r="G17" t="n">
-        <v>6.167703056293158</v>
+        <v>14119.27183211155</v>
       </c>
       <c r="H17" t="n">
         <v>10.14205855747842</v>
@@ -1068,7 +1068,7 @@
         <v>162</v>
       </c>
       <c r="G18" t="n">
-        <v>6.700187296271516</v>
+        <v>55637.16879639876</v>
       </c>
       <c r="H18" t="n">
         <v>15.17397860993796</v>
@@ -1102,7 +1102,7 @@
         <v>32</v>
       </c>
       <c r="G19" t="n">
-        <v>5.085421131685377</v>
+        <v>3888.794229338212</v>
       </c>
       <c r="H19" t="n">
         <v>4.51134982711266</v>
@@ -1136,7 +1136,7 @@
         </is>
       </c>
       <c r="G20" t="n">
-        <v>14.21049931317337</v>
+        <v>10364.95564377428</v>
       </c>
       <c r="H20" t="n">
         <v>5.038458543480214</v>
@@ -1172,7 +1172,7 @@
         </is>
       </c>
       <c r="G21" t="n">
-        <v>9.284857405438633</v>
+        <v>6149.330901430048</v>
       </c>
       <c r="H21" t="n">
         <v>3.596348206233991</v>
@@ -1206,7 +1206,7 @@
         </is>
       </c>
       <c r="G22" t="n">
-        <v>13.93271006080602</v>
+        <v>9705.761004189308</v>
       </c>
       <c r="H22" t="n">
         <v>5.455880937064808</v>
@@ -1240,7 +1240,7 @@
         <v>21</v>
       </c>
       <c r="G23" t="n">
-        <v>4.66881142969264</v>
+        <v>3104.828748281296</v>
       </c>
       <c r="H23" t="n">
         <v>3.296949999156094</v>
@@ -1276,7 +1276,7 @@
         </is>
       </c>
       <c r="G24" t="n">
-        <v>10.32897010930915</v>
+        <v>8765.273749540707</v>
       </c>
       <c r="H24" t="n">
         <v>6.082792657141333</v>
@@ -1312,7 +1312,7 @@
         </is>
       </c>
       <c r="G25" t="n">
-        <v>9.1526725352436</v>
+        <v>5997.531188087642</v>
       </c>
       <c r="H25" t="n">
         <v>4.335686055925608</v>
@@ -1346,7 +1346,7 @@
         <v>26.5</v>
       </c>
       <c r="G26" t="n">
-        <v>4.898656630433146</v>
+        <v>3474.771952143002</v>
       </c>
       <c r="H26" t="n">
         <v>2.797845948929992</v>
@@ -1382,7 +1382,7 @@
         </is>
       </c>
       <c r="G27" t="n">
-        <v>9.923203658712012</v>
+        <v>7203.821623820533</v>
       </c>
       <c r="H27" t="n">
         <v>4.906882475123913</v>
@@ -1418,7 +1418,7 @@
         </is>
       </c>
       <c r="G28" t="n">
-        <v>9.720837221341792</v>
+        <v>6809.107603285432</v>
       </c>
       <c r="H28" t="n">
         <v>5.125636172213079</v>
@@ -1454,7 +1454,7 @@
         </is>
       </c>
       <c r="G29" t="n">
-        <v>14.91009783231232</v>
+        <v>10922.02687339882</v>
       </c>
       <c r="H29" t="n">
         <v>5.673518647139566</v>
@@ -1488,7 +1488,7 @@
         </is>
       </c>
       <c r="G30" t="n">
-        <v>14.70465682730861</v>
+        <v>11316.4299963805</v>
       </c>
       <c r="H30" t="n">
         <v>5.99023766591303</v>
@@ -1522,7 +1522,7 @@
         <v>46</v>
       </c>
       <c r="G31" t="n">
-        <v>5.445641944318584</v>
+        <v>5179.15389591168</v>
       </c>
       <c r="H31" t="n">
         <v>5.99023766591303</v>
@@ -1556,7 +1556,7 @@
         <v>38</v>
       </c>
       <c r="G32" t="n">
-        <v>5.255879483850069</v>
+        <v>4396.914728577612</v>
       </c>
       <c r="H32" t="n">
         <v>5.794918654118675</v>
@@ -1590,7 +1590,7 @@
         <v>30</v>
       </c>
       <c r="G33" t="n">
-        <v>5.021469722468859</v>
+        <v>3732.821908544496</v>
       </c>
       <c r="H33" t="n">
         <v>5.705869811818438</v>
@@ -1626,7 +1626,7 @@
         </is>
       </c>
       <c r="G34" t="n">
-        <v>8.787978677346086</v>
+        <v>5687.315079624331</v>
       </c>
       <c r="H34" t="n">
         <v>1.729580387808674</v>
@@ -1660,7 +1660,7 @@
         <v>25</v>
       </c>
       <c r="G35" t="n">
-        <v>4.841024610784725</v>
+        <v>3369.713962138709</v>
       </c>
       <c r="H35" t="n">
         <v>2.191908096483702</v>
@@ -1696,7 +1696,7 @@
         </is>
       </c>
       <c r="G36" t="n">
-        <v>24.41587093407917</v>
+        <v>62321.46145534028</v>
       </c>
       <c r="H36" t="n">
         <v>12.15614658792244</v>
@@ -1730,7 +1730,7 @@
         <v>184</v>
       </c>
       <c r="G37" t="n">
-        <v>6.827317159810444</v>
+        <v>87280.98669818419</v>
       </c>
       <c r="H37" t="n">
         <v>8.75807344672109</v>
@@ -1764,7 +1764,7 @@
         <v>286</v>
       </c>
       <c r="G38" t="n">
-        <v>7.267822662086538</v>
+        <v>704015.1430638162</v>
       </c>
       <c r="H38" t="n">
         <v>17.34006374428096</v>
@@ -1798,7 +1798,7 @@
         <v>119</v>
       </c>
       <c r="G39" t="n">
-        <v>6.392347506522334</v>
+        <v>23075.15452782658</v>
       </c>
       <c r="H39" t="n">
         <v>12.83579989960463</v>
@@ -1832,7 +1832,7 @@
         <v>125</v>
       </c>
       <c r="G40" t="n">
-        <v>6.441423300967839</v>
+        <v>26090.2173846496</v>
       </c>
       <c r="H40" t="n">
         <v>14.72485170447186</v>
@@ -1868,7 +1868,7 @@
         </is>
       </c>
       <c r="G41" t="n">
-        <v>12.87406177129333</v>
+        <v>51781.74064328411</v>
       </c>
       <c r="H41" t="n">
         <v>14.72485170447186</v>
@@ -1902,7 +1902,7 @@
         <v>121</v>
       </c>
       <c r="G42" t="n">
-        <v>6.408975149416898</v>
+        <v>24039.32734200243</v>
       </c>
       <c r="H42" t="n">
         <v>14.72485170447186</v>
@@ -1936,7 +1936,7 @@
         <v>109</v>
       </c>
       <c r="G43" t="n">
-        <v>6.30479060871619</v>
+        <v>18804.25587063291</v>
       </c>
       <c r="H43" t="n">
         <v>14.72485170447186</v>
@@ -1970,7 +1970,7 @@
         <v>35</v>
       </c>
       <c r="G44" t="n">
-        <v>5.174277925338009</v>
+        <v>4135.057027827404</v>
       </c>
       <c r="H44" t="n">
         <v>4.254177487754458</v>
@@ -2004,7 +2004,7 @@
         <v>41</v>
       </c>
       <c r="G45" t="n">
-        <v>5.331321682494765</v>
+        <v>4675.354898440264</v>
       </c>
       <c r="H45" t="n">
         <v>5.629225084680439</v>
@@ -2040,7 +2040,7 @@
         </is>
       </c>
       <c r="G46" t="n">
-        <v>9.096290374666214</v>
+        <v>5980.586522585369</v>
       </c>
       <c r="H46" t="n">
         <v>4.023752878673481</v>
@@ -2076,7 +2076,7 @@
         </is>
       </c>
       <c r="G47" t="n">
-        <v>9.006481183657899</v>
+        <v>5850.854283169396</v>
       </c>
       <c r="H47" t="n">
         <v>1.899576113635789</v>
@@ -2110,7 +2110,7 @@
         <v>40</v>
       </c>
       <c r="G48" t="n">
-        <v>5.306801276196347</v>
+        <v>4580.635519804893</v>
       </c>
       <c r="H48" t="n">
         <v>2.365335151427421</v>
@@ -2144,7 +2144,7 @@
         <v>39.5</v>
       </c>
       <c r="G49" t="n">
-        <v>5.294311855187509</v>
+        <v>4533.997884238532</v>
       </c>
       <c r="H49" t="n">
         <v>7.993766563779609</v>
@@ -2178,7 +2178,7 @@
         <v>55</v>
       </c>
       <c r="G50" t="n">
-        <v>5.623327737665798</v>
+        <v>6226.70707396812</v>
       </c>
       <c r="H50" t="n">
         <v>15.84119336322231</v>
@@ -2212,7 +2212,7 @@
         <v>303</v>
       </c>
       <c r="G51" t="n">
-        <v>7.325507918554448</v>
+        <v>996993.6517086506</v>
       </c>
       <c r="H51" t="n">
         <v>23.7094888452947</v>
@@ -2246,7 +2246,7 @@
         <v>258</v>
       </c>
       <c r="G52" t="n">
-        <v>7.164898243850065</v>
+        <v>396912.0608177663</v>
       </c>
       <c r="H52" t="n">
         <v>39.9075080639763</v>
@@ -2280,7 +2280,7 @@
         <v>92</v>
       </c>
       <c r="G53" t="n">
-        <v>6.135712066398106</v>
+        <v>13278.40038327635</v>
       </c>
       <c r="H53" t="n">
         <v>11.22180954476787</v>
@@ -2314,7 +2314,7 @@
         <v>105</v>
       </c>
       <c r="G54" t="n">
-        <v>6.267502210816609</v>
+        <v>17326.0979635562</v>
       </c>
       <c r="H54" t="n">
         <v>13.78495271955164</v>
@@ -2348,7 +2348,7 @@
         <v>62</v>
       </c>
       <c r="G55" t="n">
-        <v>5.742547956002077</v>
+        <v>7185.88663877516</v>
       </c>
       <c r="H55" t="n">
         <v>9.274176842358907</v>
@@ -2414,7 +2414,7 @@
         </is>
       </c>
       <c r="G57" t="n">
-        <v>12.90663435485469</v>
+        <v>53810.08823850274</v>
       </c>
       <c r="H57" t="n">
         <v>14.02726193095983</v>
@@ -2448,7 +2448,7 @@
         <v>90</v>
       </c>
       <c r="G58" t="n">
-        <v>6.113801641722924</v>
+        <v>12745.82838227329</v>
       </c>
       <c r="H58" t="n">
         <v>10.20003749663586</v>
@@ -2482,7 +2482,7 @@
         <v>67</v>
       </c>
       <c r="G59" t="n">
-        <v>5.819765372517812</v>
+        <v>7960.211275770292</v>
       </c>
       <c r="H59" t="n">
         <v>9.008576468763605</v>
@@ -2516,7 +2516,7 @@
         <v>259</v>
       </c>
       <c r="G60" t="n">
-        <v>7.168762469194609</v>
+        <v>405119.494832326</v>
       </c>
       <c r="H60" t="n">
         <v>24.83014681626212</v>
@@ -2550,7 +2550,7 @@
         <v>204</v>
       </c>
       <c r="G61" t="n">
-        <v>6.930350082953777</v>
+        <v>131430.6268666013</v>
       </c>
       <c r="H61" t="n">
         <v>24.58724845104962</v>
@@ -2586,7 +2586,7 @@
         </is>
       </c>
       <c r="G62" t="n">
-        <v>18.27354515187801</v>
+        <v>12557.29540260998</v>
       </c>
       <c r="H62" t="n">
         <v>5.968240341152113</v>
@@ -2622,7 +2622,7 @@
         </is>
       </c>
       <c r="G63" t="n">
-        <v>18.64817697233678</v>
+        <v>12522.01418938059</v>
       </c>
       <c r="H63" t="n">
         <v>5.473181392530233</v>
@@ -2656,7 +2656,7 @@
         <v>53</v>
       </c>
       <c r="G64" t="n">
-        <v>5.586480573236176</v>
+        <v>5976.965407026083</v>
       </c>
       <c r="H64" t="n">
         <v>5.378650973312014</v>
@@ -2690,7 +2690,7 @@
         <v>66.5</v>
       </c>
       <c r="G65" t="n">
-        <v>5.81230648119604</v>
+        <v>7879.164567097337</v>
       </c>
       <c r="H65" t="n">
         <v>8.915391336980173</v>
@@ -2724,7 +2724,7 @@
         <v>68</v>
       </c>
       <c r="G66" t="n">
-        <v>5.834518296645255</v>
+        <v>8124.814257733681</v>
       </c>
       <c r="H66" t="n">
         <v>14.36635505845379</v>
@@ -2758,7 +2758,7 @@
         <v>56</v>
       </c>
       <c r="G67" t="n">
-        <v>5.641254375709414</v>
+        <v>6355.464278605056</v>
       </c>
       <c r="H67" t="n">
         <v>12.27465026375843</v>
@@ -2792,7 +2792,7 @@
         <v>56</v>
       </c>
       <c r="G68" t="n">
-        <v>5.641254375709414</v>
+        <v>6355.464278605056</v>
       </c>
       <c r="H68" t="n">
         <v>9.554363062374231</v>
@@ -2826,7 +2826,7 @@
         <v>55</v>
       </c>
       <c r="G69" t="n">
-        <v>5.623327737665798</v>
+        <v>6226.70707396812</v>
       </c>
       <c r="H69" t="n">
         <v>6.282734232682529</v>
@@ -2860,7 +2860,7 @@
         <v>58</v>
       </c>
       <c r="G70" t="n">
-        <v>5.676171440948019</v>
+        <v>6621.021151539858</v>
       </c>
       <c r="H70" t="n">
         <v>6.414241425995747</v>
@@ -2894,7 +2894,7 @@
         <v>77</v>
       </c>
       <c r="G71" t="n">
-        <v>5.958329081223977</v>
+        <v>9768.166660048983</v>
       </c>
       <c r="H71" t="n">
         <v>7.727327806808214</v>
@@ -2928,7 +2928,7 @@
         <v>75</v>
       </c>
       <c r="G72" t="n">
-        <v>5.932109899782458</v>
+        <v>9376.383620367058</v>
       </c>
       <c r="H72" t="n">
         <v>7.178911038920171</v>
@@ -2964,7 +2964,7 @@
         </is>
       </c>
       <c r="G73" t="n">
-        <v>24.52522101501422</v>
+        <v>54675.26391817947</v>
       </c>
       <c r="H73" t="n">
         <v>18.56667120974419</v>
@@ -2998,7 +2998,7 @@
         <v>73</v>
       </c>
       <c r="G74" t="n">
-        <v>5.905184720651817</v>
+        <v>9000.314271444548</v>
       </c>
       <c r="H74" t="n">
         <v>13.10814149589888</v>
@@ -3032,7 +3032,7 @@
         <v>73</v>
       </c>
       <c r="G75" t="n">
-        <v>5.905184720651817</v>
+        <v>9000.314271444548</v>
       </c>
       <c r="H75" t="n">
         <v>12.69023763497751</v>
@@ -3068,7 +3068,7 @@
         </is>
       </c>
       <c r="G76" t="n">
-        <v>19.26180204306857</v>
+        <v>75526.37863574187</v>
       </c>
       <c r="H76" t="n">
         <v>20.84367227262954</v>
@@ -3104,7 +3104,7 @@
         </is>
       </c>
       <c r="G77" t="n">
-        <v>12.58983062141782</v>
+        <v>36970.14257760406</v>
       </c>
       <c r="H77" t="n">
         <v>15.66787827369098</v>
@@ -3140,7 +3140,7 @@
         </is>
       </c>
       <c r="G78" t="n">
-        <v>12.07642099395054</v>
+        <v>22373.50031626973</v>
       </c>
       <c r="H78" t="n">
         <v>19.71760208653519</v>
@@ -3176,7 +3176,7 @@
         </is>
       </c>
       <c r="G79" t="n">
-        <v>12.11060621500734</v>
+        <v>30449.98165665026</v>
       </c>
       <c r="H79" t="n">
         <v>16.40397530407548</v>
@@ -3210,7 +3210,7 @@
         <v>55</v>
       </c>
       <c r="G80" t="n">
-        <v>5.623327737665798</v>
+        <v>6226.70707396812</v>
       </c>
       <c r="H80" t="n">
         <v>9.54047478223722</v>
@@ -3244,7 +3244,7 @@
         <v>63</v>
       </c>
       <c r="G81" t="n">
-        <v>5.758475815662073</v>
+        <v>7334.477967298512</v>
       </c>
       <c r="H81" t="n">
         <v>8.740869835132035</v>
@@ -3280,7 +3280,7 @@
         </is>
       </c>
       <c r="G82" t="n">
-        <v>11.19086275357465</v>
+        <v>12082.5833954004</v>
       </c>
       <c r="H82" t="n">
         <v>6.433726928794039</v>
@@ -3314,7 +3314,7 @@
         </is>
       </c>
       <c r="G83" t="n">
-        <v>31.83277156844789</v>
+        <v>20853.71659514599</v>
       </c>
       <c r="H83" t="n">
         <v>4.705307922833859</v>
@@ -3350,7 +3350,7 @@
         </is>
       </c>
       <c r="G84" t="n">
-        <v>19.94380666817378</v>
+        <v>15558.71669900454</v>
       </c>
       <c r="H84" t="n">
         <v>3.272469962821916</v>
@@ -3386,7 +3386,7 @@
         </is>
       </c>
       <c r="G85" t="n">
-        <v>33.3931812949407</v>
+        <v>42448.35294930259</v>
       </c>
       <c r="H85" t="n">
         <v>10.42483387224127</v>
@@ -3420,7 +3420,7 @@
         <v>124</v>
       </c>
       <c r="G86" t="n">
-        <v>6.433409435956624</v>
+        <v>25561.64806043415</v>
       </c>
       <c r="H86" t="n">
         <v>8.108691082271754</v>
@@ -3456,7 +3456,7 @@
         </is>
       </c>
       <c r="G87" t="n">
-        <v>18.27165567281002</v>
+        <v>12010.38312791689</v>
       </c>
       <c r="H87" t="n">
         <v>5.473921767177792</v>
@@ -3490,7 +3490,7 @@
         <v>29.7</v>
       </c>
       <c r="G88" t="n">
-        <v>5.011514241042526</v>
+        <v>3709.971867705583</v>
       </c>
       <c r="H88" t="n">
         <v>9.064858939911851</v>
@@ -3524,7 +3524,7 @@
         <v>39.5</v>
       </c>
       <c r="G89" t="n">
-        <v>5.294311855187509</v>
+        <v>4533.997884238532</v>
       </c>
       <c r="H89" t="n">
         <v>9.197856377128165</v>
@@ -3558,7 +3558,7 @@
         </is>
       </c>
       <c r="G90" t="n">
-        <v>10.17303159483335</v>
+        <v>7907.42890030647</v>
       </c>
       <c r="H90" t="n">
         <v>15.75200100995447</v>
@@ -3592,7 +3592,7 @@
         </is>
       </c>
       <c r="G91" t="n">
-        <v>10.37672492297533</v>
+        <v>8504.854813555125</v>
       </c>
       <c r="H91" t="n">
         <v>15.56229393431864</v>
@@ -3626,7 +3626,7 @@
         </is>
       </c>
       <c r="G92" t="n">
-        <v>9.993933083782991</v>
+        <v>8054.527734701296</v>
       </c>
       <c r="H92" t="n">
         <v>13.6864900164287</v>
@@ -3660,7 +3660,7 @@
         </is>
       </c>
       <c r="G93" t="n">
-        <v>10.18661388675342</v>
+        <v>8020.029160951616</v>
       </c>
       <c r="H93" t="n">
         <v>14.00468264936305</v>
@@ -3694,7 +3694,7 @@
         </is>
       </c>
       <c r="G94" t="n">
-        <v>10.4316368720554</v>
+        <v>8528.398987949713</v>
       </c>
       <c r="H94" t="n">
         <v>9.618841920801845</v>
@@ -3728,7 +3728,7 @@
         </is>
       </c>
       <c r="G95" t="n">
-        <v>15.03550920006403</v>
+        <v>12228.05441493991</v>
       </c>
       <c r="H95" t="n">
         <v>8.58591978534246</v>
@@ -3762,7 +3762,7 @@
         </is>
       </c>
       <c r="G96" t="n">
-        <v>14.96560561159958</v>
+        <v>11209.68933226864</v>
       </c>
       <c r="H96" t="n">
         <v>12.88934151197478</v>
@@ -3796,7 +3796,7 @@
         </is>
       </c>
       <c r="G97" t="n">
-        <v>9.179785764270914</v>
+        <v>6581.450688825977</v>
       </c>
       <c r="H97" t="n">
         <v>29.27741167994195</v>
@@ -3830,7 +3830,7 @@
         </is>
       </c>
       <c r="G98" t="n">
-        <v>9.7156609347012</v>
+        <v>7031.583529618736</v>
       </c>
       <c r="H98" t="n">
         <v>20.66228460699256</v>
@@ -3862,7 +3862,7 @@
         <v>179</v>
       </c>
       <c r="G99" t="n">
-        <v>6.799810315402893</v>
+        <v>78790.78260682251</v>
       </c>
       <c r="H99" t="n">
         <v>23.8350718518842</v>
@@ -3896,7 +3896,7 @@
         <v>240</v>
       </c>
       <c r="G100" t="n">
-        <v>7.092660162778362</v>
+        <v>274596.5376651874</v>
       </c>
       <c r="H100" t="n">
         <v>37.61452930692663</v>
@@ -3932,7 +3932,7 @@
         </is>
       </c>
       <c r="G101" t="n">
-        <v>24.85325988675162</v>
+        <v>76441.48363027762</v>
       </c>
       <c r="H101" t="n">
         <v>25.59883264386158</v>
@@ -3966,7 +3966,7 @@
         <v>217</v>
       </c>
       <c r="G102" t="n">
-        <v>6.992044036337617</v>
+        <v>171495.0484073638</v>
       </c>
       <c r="H102" t="n">
         <v>32.00669058082102</v>
@@ -4000,7 +4000,7 @@
         <v>291</v>
       </c>
       <c r="G103" t="n">
-        <v>7.285137049149095</v>
+        <v>779877.2179190471</v>
       </c>
       <c r="H103" t="n">
         <v>22.49552978615448</v>
@@ -4034,7 +4034,7 @@
         <v>308</v>
       </c>
       <c r="G104" t="n">
-        <v>7.341859672854985</v>
+        <v>1104426.009920377</v>
       </c>
       <c r="H104" t="n">
         <v>18.18052886241581</v>
@@ -4070,7 +4070,7 @@
         </is>
       </c>
       <c r="G105" t="n">
-        <v>12.9478532359659</v>
+        <v>73182.24835141651</v>
       </c>
       <c r="H105" t="n">
         <v>14.56268612901544</v>
@@ -4104,7 +4104,7 @@
         <v>217</v>
       </c>
       <c r="G106" t="n">
-        <v>6.992044036337617</v>
+        <v>171495.0484073638</v>
       </c>
       <c r="H106" t="n">
         <v>19.6243219559596</v>
@@ -4138,7 +4138,7 @@
         <v>175</v>
       </c>
       <c r="G107" t="n">
-        <v>6.777246741495336</v>
+        <v>72597.22625892558</v>
       </c>
       <c r="H107" t="n">
         <v>20.39110905670868</v>
@@ -4172,7 +4172,7 @@
         <v>331</v>
       </c>
       <c r="G108" t="n">
-        <v>7.413814159859278</v>
+        <v>1768398.337141099</v>
       </c>
       <c r="H108" t="n">
         <v>21.15559715542659</v>
@@ -4206,7 +4206,7 @@
         <v>82</v>
       </c>
       <c r="G109" t="n">
-        <v>6.021018494968811</v>
+        <v>10820.74826665774</v>
       </c>
       <c r="H109" t="n">
         <v>8.954695792840937</v>
@@ -4240,7 +4240,7 @@
         <v>76</v>
       </c>
       <c r="G110" t="n">
-        <v>5.945305418726402</v>
+        <v>9570.270522419889</v>
       </c>
       <c r="H110" t="n">
         <v>6.452785228463761</v>
@@ -4276,7 +4276,7 @@
         </is>
       </c>
       <c r="G111" t="n">
-        <v>11.68628812536009</v>
+        <v>17628.34695221426</v>
       </c>
       <c r="H111" t="n">
         <v>5.877842795278028</v>
@@ -4312,7 +4312,7 @@
         </is>
       </c>
       <c r="G112" t="n">
-        <v>11.55766587948578</v>
+        <v>15947.12034412665</v>
       </c>
       <c r="H112" t="n">
         <v>4.898202329398357</v>
@@ -4348,7 +4348,7 @@
         </is>
       </c>
       <c r="G113" t="n">
-        <v>10.47118100781044</v>
+        <v>8741.240468143069</v>
       </c>
       <c r="H113" t="n">
         <v>3.647753961709322</v>
@@ -4384,7 +4384,7 @@
         </is>
       </c>
       <c r="G114" t="n">
-        <v>21.34048284828347</v>
+        <v>18827.60510363356</v>
       </c>
       <c r="H114" t="n">
         <v>3.683691348572317</v>
@@ -4420,7 +4420,7 @@
         </is>
       </c>
       <c r="G115" t="n">
-        <v>16.15751239530749</v>
+        <v>15275.6021962807</v>
       </c>
       <c r="H115" t="n">
         <v>7.837123727037371</v>
@@ -4456,7 +4456,7 @@
         </is>
       </c>
       <c r="G116" t="n">
-        <v>16.81909477446257</v>
+        <v>28770.75494674456</v>
       </c>
       <c r="H116" t="n">
         <v>16.67200337294842</v>
@@ -4492,7 +4492,7 @@
         </is>
       </c>
       <c r="G117" t="n">
-        <v>17.39916879563044</v>
+        <v>27168.23711901997</v>
       </c>
       <c r="H117" t="n">
         <v>11.67172045073898</v>
@@ -4528,7 +4528,7 @@
         </is>
       </c>
       <c r="G118" t="n">
-        <v>29.00544056461824</v>
+        <v>39692.5425913302</v>
       </c>
       <c r="H118" t="n">
         <v>6.663143657335704</v>
@@ -4564,7 +4564,7 @@
         </is>
       </c>
       <c r="G119" t="n">
-        <v>14.77479378416899</v>
+        <v>10619.11761601442</v>
       </c>
       <c r="H119" t="n">
         <v>3.765282013823312</v>
@@ -4600,7 +4600,7 @@
         </is>
       </c>
       <c r="G120" t="n">
-        <v>13.60090841532846</v>
+        <v>8821.365188703106</v>
       </c>
       <c r="H120" t="n">
         <v>3.397019644574772</v>
@@ -4664,7 +4664,7 @@
         <v>93</v>
       </c>
       <c r="G122" t="n">
-        <v>6.146489844345901</v>
+        <v>13552.97403755158</v>
       </c>
       <c r="H122" t="n">
         <v>16.67200337294842</v>
@@ -4698,7 +4698,7 @@
         <v>130</v>
       </c>
       <c r="G123" t="n">
-        <v>6.480556700699851</v>
+        <v>28901.60296878623</v>
       </c>
       <c r="H123" t="n">
         <v>20.01493418204281</v>
@@ -4732,7 +4732,7 @@
         <v>117</v>
       </c>
       <c r="G124" t="n">
-        <v>6.375438703502036</v>
+        <v>22149.65289618294</v>
       </c>
       <c r="H124" t="n">
         <v>17.27054595242531</v>
@@ -4766,7 +4766,7 @@
         <v>135</v>
       </c>
       <c r="G125" t="n">
-        <v>6.518216176124221</v>
+        <v>32015.9330928692</v>
       </c>
       <c r="H125" t="n">
         <v>21.0006718959081</v>
@@ -4800,7 +4800,7 @@
         <v>129</v>
       </c>
       <c r="G126" t="n">
-        <v>6.472851576407184</v>
+        <v>28316.07696397258</v>
       </c>
       <c r="H126" t="n">
         <v>20.01493418204281</v>
@@ -4834,7 +4834,7 @@
         <v>115</v>
       </c>
       <c r="G127" t="n">
-        <v>6.358239068187844</v>
+        <v>21261.27141769553</v>
       </c>
       <c r="H127" t="n">
         <v>19.46322089377813</v>
@@ -4868,7 +4868,7 @@
         <v>90</v>
       </c>
       <c r="G128" t="n">
-        <v>6.113801641722924</v>
+        <v>12745.82838227329</v>
       </c>
       <c r="H128" t="n">
         <v>16.67200337294842</v>
@@ -4902,7 +4902,7 @@
         <v>131</v>
       </c>
       <c r="G129" t="n">
-        <v>6.488202909712459</v>
+        <v>29499.23660781597</v>
       </c>
       <c r="H129" t="n">
         <v>15.90939605656152</v>
@@ -4936,7 +4936,7 @@
         <v>87</v>
       </c>
       <c r="G130" t="n">
-        <v>6.080008707118627</v>
+        <v>11986.75218444618</v>
       </c>
       <c r="H130" t="n">
         <v>17.46431724156258</v>
@@ -4970,7 +4970,7 @@
         <v>62</v>
       </c>
       <c r="G131" t="n">
-        <v>5.742547956002077</v>
+        <v>7185.88663877516</v>
       </c>
       <c r="H131" t="n">
         <v>13.37288425104356</v>
@@ -5004,7 +5004,7 @@
         <v>80</v>
       </c>
       <c r="G132" t="n">
-        <v>5.996412286831915</v>
+        <v>10386.74813182355</v>
       </c>
       <c r="H132" t="n">
         <v>4.752049538775145</v>
@@ -5040,7 +5040,7 @@
         </is>
       </c>
       <c r="G133" t="n">
-        <v>48.30082693397208</v>
+        <v>35028.74799406027</v>
       </c>
       <c r="H133" t="n">
         <v>4.215844115381171</v>
@@ -5074,7 +5074,7 @@
         <v>41.7</v>
       </c>
       <c r="G134" t="n">
-        <v>5.348135097827601</v>
+        <v>4742.82145334331</v>
       </c>
       <c r="H134" t="n">
         <v>5.521168820224332</v>
@@ -5110,7 +5110,7 @@
         </is>
       </c>
       <c r="G135" t="n">
-        <v>11.80869224629213</v>
+        <v>18034.57221535529</v>
       </c>
       <c r="H135" t="n">
         <v>9.628065938662099</v>
@@ -5146,7 +5146,7 @@
         </is>
       </c>
       <c r="G136" t="n">
-        <v>20.75137304814415</v>
+        <v>17543.85063789346</v>
       </c>
       <c r="H136" t="n">
         <v>7.98444184339372</v>
@@ -5182,7 +5182,7 @@
         </is>
       </c>
       <c r="G137" t="n">
-        <v>27.23095574782436</v>
+        <v>27644.3007201818</v>
       </c>
       <c r="H137" t="n">
         <v>7.107986283200214</v>
@@ -5218,7 +5218,7 @@
         </is>
       </c>
       <c r="G138" t="n">
-        <v>20.10453827107946</v>
+        <v>15028.47880948078</v>
       </c>
       <c r="H138" t="n">
         <v>5.062727414011374</v>
@@ -5252,7 +5252,7 @@
         <v>54.5</v>
       </c>
       <c r="G139" t="n">
-        <v>5.614242448781546</v>
+        <v>6163.309998597545</v>
       </c>
       <c r="H139" t="n">
         <v>7.057961884250789</v>
@@ -5288,7 +5288,7 @@
         </is>
       </c>
       <c r="G140" t="n">
-        <v>15.27994616628515</v>
+        <v>12200.18223936939</v>
       </c>
       <c r="H140" t="n">
         <v>6.154340955627815</v>
@@ -5322,7 +5322,7 @@
         <v>81</v>
       </c>
       <c r="G141" t="n">
-        <v>6.008791072175986</v>
+        <v>10601.52757123425</v>
       </c>
       <c r="H141" t="n">
         <v>5.267169095163338</v>
@@ -5356,7 +5356,7 @@
         <v>58.9</v>
       </c>
       <c r="G142" t="n">
-        <v>5.691494958044276</v>
+        <v>6744.114534092521</v>
       </c>
       <c r="H142" t="n">
         <v>7.899484278999021</v>
@@ -5390,7 +5390,7 @@
         <v>51.3</v>
       </c>
       <c r="G143" t="n">
-        <v>5.554056270164168</v>
+        <v>5772.576579868776</v>
       </c>
       <c r="H143" t="n">
         <v>6.246920984795349</v>
@@ -5424,7 +5424,7 @@
         <v>47.3</v>
       </c>
       <c r="G144" t="n">
-        <v>5.473341948391249</v>
+        <v>5318.808040744359</v>
       </c>
       <c r="H144" t="n">
         <v>6.0684849285739</v>
@@ -5458,7 +5458,7 @@
         <v>44.7</v>
       </c>
       <c r="G145" t="n">
-        <v>5.417152737194565</v>
+        <v>5043.1666027532</v>
       </c>
       <c r="H145" t="n">
         <v>5.928368238315379</v>
@@ -5492,7 +5492,7 @@
         <v>25.2</v>
       </c>
       <c r="G146" t="n">
-        <v>4.848903505702014</v>
+        <v>3383.53603955737</v>
       </c>
       <c r="H146" t="n">
         <v>2.074861749752159</v>
@@ -5526,7 +5526,7 @@
         <v>57</v>
       </c>
       <c r="G147" t="n">
-        <v>5.658865300768017</v>
+        <v>6486.883952754216</v>
       </c>
       <c r="H147" t="n">
         <v>6.075083888251274</v>
@@ -5560,7 +5560,7 @@
         <v>50.6</v>
       </c>
       <c r="G148" t="n">
-        <v>5.540393362737931</v>
+        <v>5690.461775719187</v>
       </c>
       <c r="H148" t="n">
         <v>6.699407308634797</v>
@@ -5596,7 +5596,7 @@
         </is>
       </c>
       <c r="G149" t="n">
-        <v>10.07148922220001</v>
+        <v>7819.098459001754</v>
       </c>
       <c r="H149" t="n">
         <v>5.954127946652007</v>
@@ -5630,7 +5630,7 @@
         <v>63.7</v>
       </c>
       <c r="G150" t="n">
-        <v>5.769476265712425</v>
+        <v>7440.316341328899</v>
       </c>
       <c r="H150" t="n">
         <v>7.517360534650028</v>
@@ -5664,7 +5664,7 @@
         <v>48.9</v>
       </c>
       <c r="G151" t="n">
-        <v>5.506413470754946</v>
+        <v>5495.870251572918</v>
       </c>
       <c r="H151" t="n">
         <v>7.080364123699438</v>
@@ -5696,7 +5696,7 @@
         <v>97.5</v>
       </c>
       <c r="G152" t="n">
-        <v>6.19360200725378</v>
+        <v>14860.53401388869</v>
       </c>
       <c r="H152" t="n">
         <v>12.14885607150393</v>
@@ -5730,7 +5730,7 @@
         <v>87</v>
       </c>
       <c r="G153" t="n">
-        <v>6.080008707118627</v>
+        <v>11986.75218444618</v>
       </c>
       <c r="H153" t="n">
         <v>14.21329207799613</v>
@@ -5764,7 +5764,7 @@
         <v>65</v>
       </c>
       <c r="G154" t="n">
-        <v>5.789590071838004</v>
+        <v>7640.941971849962</v>
       </c>
       <c r="H154" t="n">
         <v>9.576564013118725</v>
@@ -5798,7 +5798,7 @@
         <v>90</v>
       </c>
       <c r="G155" t="n">
-        <v>6.113801641722924</v>
+        <v>12745.82838227329</v>
       </c>
       <c r="H155" t="n">
         <v>8.609374360498016</v>
@@ -5832,7 +5832,7 @@
         <v>69</v>
       </c>
       <c r="G156" t="n">
-        <v>5.849056732497973</v>
+        <v>8292.820935997644</v>
       </c>
       <c r="H156" t="n">
         <v>12</v>
@@ -5866,7 +5866,7 @@
         <v>72</v>
       </c>
       <c r="G157" t="n">
-        <v>5.891445297015908</v>
+        <v>8817.974279330003</v>
       </c>
       <c r="H157" t="n">
         <v>10.45613718524691</v>
@@ -5900,7 +5900,7 @@
         <v>38.2</v>
       </c>
       <c r="G158" t="n">
-        <v>5.261089945467491</v>
+        <v>4414.950234399322</v>
       </c>
       <c r="H158" t="n">
         <v>4.739440985157887</v>
@@ -5932,7 +5932,7 @@
         <v>29.8</v>
       </c>
       <c r="G159" t="n">
-        <v>5.014843759403572</v>
+        <v>3717.572964006365</v>
       </c>
       <c r="H159" t="n">
         <v>4.849310761891133</v>
@@ -5964,7 +5964,7 @@
         <v>34</v>
       </c>
       <c r="G160" t="n">
-        <v>5.145527427160102</v>
+        <v>4051.283701351525</v>
       </c>
       <c r="H160" t="n">
         <v>5.125636172213079</v>
@@ -5996,7 +5996,7 @@
         <v>37</v>
       </c>
       <c r="G161" t="n">
-        <v>5.229411991233183</v>
+        <v>4307.836350561312</v>
       </c>
       <c r="H161" t="n">
         <v>5.913995913412071</v>
@@ -6030,7 +6030,7 @@
         <v>48</v>
       </c>
       <c r="G162" t="n">
-        <v>5.48794549852443</v>
+        <v>5395.559787401999</v>
       </c>
       <c r="H162" t="n">
         <v>5.150142966599134</v>
@@ -6064,7 +6064,7 @@
         <v>90</v>
       </c>
       <c r="G163" t="n">
-        <v>6.113801641722924</v>
+        <v>12745.82838227329</v>
       </c>
       <c r="H163" t="n">
         <v>14.65523870026262</v>
@@ -6098,7 +6098,7 @@
         <v>81</v>
       </c>
       <c r="G164" t="n">
-        <v>6.008791072175986</v>
+        <v>10601.52757123425</v>
       </c>
       <c r="H164" t="n">
         <v>11.58314874693474</v>
@@ -6132,7 +6132,7 @@
         <v>71</v>
       </c>
       <c r="G165" t="n">
-        <v>5.877514468776316</v>
+        <v>8639.328366302194</v>
       </c>
       <c r="H165" t="n">
         <v>6.725986983296809</v>
@@ -6168,7 +6168,7 @@
         </is>
       </c>
       <c r="G166" t="n">
-        <v>11.14408551709347</v>
+        <v>12876.46841640035</v>
       </c>
       <c r="H166" t="n">
         <v>7.721921541004152</v>
@@ -6202,7 +6202,7 @@
         <v>42.5</v>
       </c>
       <c r="G167" t="n">
-        <v>5.367010526459294</v>
+        <v>4821.119017800447</v>
       </c>
       <c r="H167" t="n">
         <v>7.496036614502667</v>
@@ -6234,7 +6234,7 @@
         <v>66.5</v>
       </c>
       <c r="G168" t="n">
-        <v>5.81230648119604</v>
+        <v>7879.164567097337</v>
       </c>
       <c r="H168" t="n">
         <v>4.747677705264452</v>
@@ -6270,7 +6270,7 @@
         </is>
       </c>
       <c r="G169" t="n">
-        <v>70.44700106670727</v>
+        <v>48635.94860038623</v>
       </c>
       <c r="H169" t="n">
         <v>6.76137237165228</v>
@@ -6306,7 +6306,7 @@
         </is>
       </c>
       <c r="G170" t="n">
-        <v>36.57430001243439</v>
+        <v>24351.66108142551</v>
       </c>
       <c r="H170" t="n">
         <v>4.503380067744351</v>
@@ -6340,7 +6340,7 @@
         <v>32.5</v>
       </c>
       <c r="G171" t="n">
-        <v>5.100789781889402</v>
+        <v>3928.795167294297</v>
       </c>
       <c r="H171" t="n">
         <v>6.547929111610984</v>
@@ -6374,7 +6374,7 @@
         <v>53</v>
       </c>
       <c r="G172" t="n">
-        <v>5.586480573236176</v>
+        <v>5976.965407026083</v>
       </c>
       <c r="H172" t="n">
         <v>13.17911296190628</v>
@@ -6408,7 +6408,7 @@
         <v>45</v>
       </c>
       <c r="G173" t="n">
-        <v>5.423799576241895</v>
+        <v>5074.227906434086</v>
       </c>
       <c r="H173" t="n">
         <v>10.4863469538792</v>
@@ -6442,7 +6442,7 @@
         <v>38</v>
       </c>
       <c r="G174" t="n">
-        <v>5.255879483850069</v>
+        <v>4396.914728577612</v>
       </c>
       <c r="H174" t="inlineStr"/>
       <c r="I174" t="n">
@@ -6536,7 +6536,7 @@
         </is>
       </c>
       <c r="G177" t="n">
-        <v>11.67435258784401</v>
+        <v>17399.96633395788</v>
       </c>
       <c r="H177" t="n">
         <v>8.954343106844133</v>
@@ -6570,7 +6570,7 @@
         <v>125.3</v>
       </c>
       <c r="G178" t="n">
-        <v>6.443814990477335</v>
+        <v>26250.90931278113</v>
       </c>
       <c r="H178" t="n">
         <v>13.32294427296602</v>
@@ -6604,7 +6604,7 @@
         <v>177.6</v>
       </c>
       <c r="G179" t="n">
-        <v>6.791970844790643</v>
+        <v>76565.13083484342</v>
       </c>
       <c r="H179" t="n">
         <v>26.15627688118688</v>
@@ -6638,7 +6638,7 @@
         <v>103.5</v>
       </c>
       <c r="G180" t="n">
-        <v>6.253152621472004</v>
+        <v>16802.25206755543</v>
       </c>
       <c r="H180" t="n">
         <v>11.40540834702391</v>
@@ -6672,7 +6672,7 @@
         <v>83.5</v>
       </c>
       <c r="G181" t="n">
-        <v>6.039083787918909</v>
+        <v>11158.10807701861</v>
       </c>
       <c r="H181" t="n">
         <v>16.23101803215132</v>
@@ -6706,7 +6706,7 @@
         <v>92.8</v>
       </c>
       <c r="G182" t="n">
-        <v>6.144343561568614</v>
+        <v>13497.60880596837</v>
       </c>
       <c r="H182" t="n">
         <v>10.55299647040566</v>
@@ -6742,7 +6742,7 @@
         </is>
       </c>
       <c r="G183" t="n">
-        <v>12.66616108364348</v>
+        <v>40275.66092126572</v>
       </c>
       <c r="H183" t="n">
         <v>15.50932567645019</v>
@@ -6776,7 +6776,7 @@
         <v>92.5</v>
       </c>
       <c r="G184" t="n">
-        <v>6.141115475363914</v>
+        <v>13414.98474299391</v>
       </c>
       <c r="H184" t="n">
         <v>14.02726193095983</v>
@@ -6810,7 +6810,7 @@
         <v>117.5</v>
       </c>
       <c r="G185" t="n">
-        <v>6.379692783552073</v>
+        <v>22377.48878540657</v>
       </c>
       <c r="H185" t="n">
         <v>18.37155042834553</v>
@@ -6844,7 +6844,7 @@
         <v>71.3</v>
       </c>
       <c r="G186" t="n">
-        <v>5.881714132148762</v>
+        <v>8692.538744447977</v>
       </c>
       <c r="H186" t="n">
         <v>15.33252242007791</v>
@@ -6878,7 +6878,7 @@
         <v>127</v>
       </c>
       <c r="G187" t="n">
-        <v>6.457260900668611</v>
+        <v>27180.37165806446</v>
       </c>
       <c r="H187" t="n">
         <v>16.40704568412136</v>
@@ -6912,7 +6912,7 @@
         <v>173</v>
       </c>
       <c r="G188" t="n">
-        <v>6.765771119310083</v>
+        <v>69685.48621946402</v>
       </c>
       <c r="H188" t="n">
         <v>20.01493418204281</v>
@@ -6948,7 +6948,7 @@
         </is>
       </c>
       <c r="G189" t="n">
-        <v>18.97242652088298</v>
+        <v>62430.4078826015</v>
       </c>
       <c r="H189" t="n">
         <v>15.94812320775646</v>
@@ -6982,7 +6982,7 @@
         <v>170</v>
       </c>
       <c r="G190" t="n">
-        <v>6.748306924557546</v>
+        <v>65535.37589813157</v>
       </c>
       <c r="H190" t="n">
         <v>19.82175381463626</v>
@@ -7016,7 +7016,7 @@
         <v>141.3</v>
       </c>
       <c r="G191" t="n">
-        <v>6.56373295202441</v>
+        <v>36422.17672568452</v>
       </c>
       <c r="H191" t="n">
         <v>7.370605914090421</v>
@@ -7052,7 +7052,7 @@
         </is>
       </c>
       <c r="G192" t="n">
-        <v>18.42733629412584</v>
+        <v>47057.39969499506</v>
       </c>
       <c r="H192" t="n">
         <v>6.516184505751228</v>
@@ -7086,7 +7086,7 @@
         <v>151</v>
       </c>
       <c r="G193" t="n">
-        <v>6.629998454560702</v>
+        <v>44420.93640460757</v>
       </c>
       <c r="H193" t="n">
         <v>12.68996955153729</v>
@@ -7122,7 +7122,7 @@
         </is>
       </c>
       <c r="G194" t="n">
-        <v>42.36181009528663</v>
+        <v>94567.171310024</v>
       </c>
       <c r="H194" t="n">
         <v>10.40944879000231</v>
@@ -7158,7 +7158,7 @@
         </is>
       </c>
       <c r="G195" t="n">
-        <v>29.28830453643562</v>
+        <v>47343.36694605261</v>
       </c>
       <c r="H195" t="n">
         <v>7.972930777453313</v>
@@ -7194,7 +7194,7 @@
         </is>
       </c>
       <c r="G196" t="n">
-        <v>23.3452804729414</v>
+        <v>33097.30121324343</v>
       </c>
       <c r="H196" t="n">
         <v>8.011963326177924</v>
@@ -7230,7 +7230,7 @@
         </is>
       </c>
       <c r="G197" t="n">
-        <v>12.38126265888695</v>
+        <v>30166.37967878635</v>
       </c>
       <c r="H197" t="n">
         <v>9.503248678973984</v>
@@ -7266,7 +7266,7 @@
         </is>
       </c>
       <c r="G198" t="n">
-        <v>8.295344890902424</v>
+        <v>5359.783040696411</v>
       </c>
       <c r="H198" t="n">
         <v>3.493982735042525</v>
@@ -7300,7 +7300,7 @@
         <v>21</v>
       </c>
       <c r="G199" t="n">
-        <v>4.66881142969264</v>
+        <v>3104.828748281296</v>
       </c>
       <c r="H199" t="n">
         <v>3.374463996958158</v>
@@ -7334,7 +7334,7 @@
         <v>25</v>
       </c>
       <c r="G200" t="n">
-        <v>4.841024610784725</v>
+        <v>3369.713962138709</v>
       </c>
       <c r="H200" t="n">
         <v>4.954407443435853</v>
@@ -7368,7 +7368,7 @@
         <v>27</v>
       </c>
       <c r="G201" t="n">
-        <v>4.917152110983285</v>
+        <v>3510.514171728857</v>
       </c>
       <c r="H201" t="n">
         <v>4.954407443435853</v>
@@ -7402,7 +7402,7 @@
         <v>44</v>
       </c>
       <c r="G202" t="n">
-        <v>5.401469445403479</v>
+        <v>4971.427643183046</v>
       </c>
       <c r="H202" t="n">
         <v>5.984904429010897</v>
@@ -7436,7 +7436,7 @@
         <v>37</v>
       </c>
       <c r="G203" t="n">
-        <v>5.229411991233183</v>
+        <v>4307.836350561312</v>
       </c>
       <c r="H203" t="n">
         <v>6.460386150037829</v>
@@ -7470,7 +7470,7 @@
         <v>33</v>
       </c>
       <c r="G204" t="n">
-        <v>5.115925807303968</v>
+        <v>3969.20756313244</v>
       </c>
       <c r="H204" t="n">
         <v>1.905964781614191</v>
@@ -7504,7 +7504,7 @@
         <v>43</v>
       </c>
       <c r="G205" t="n">
-        <v>5.378629268754704</v>
+        <v>4870.710040450867</v>
       </c>
       <c r="H205" t="n">
         <v>6.630625411594059</v>
@@ -7538,7 +7538,7 @@
         <v>48</v>
       </c>
       <c r="G206" t="n">
-        <v>5.48794549852443</v>
+        <v>5395.559787401999</v>
       </c>
       <c r="H206" t="n">
         <v>7.675453536720804</v>
@@ -7574,7 +7574,7 @@
         </is>
       </c>
       <c r="G207" t="n">
-        <v>46.04534379752437</v>
+        <v>29624.91045733112</v>
       </c>
       <c r="H207" t="n">
         <v>5.077133059428725</v>
@@ -7610,7 +7610,7 @@
         </is>
       </c>
       <c r="G208" t="n">
-        <v>14.72609548857594</v>
+        <v>10503.11704906639</v>
       </c>
       <c r="H208" t="n">
         <v>3.540182061849719</v>
@@ -7646,7 +7646,7 @@
         </is>
       </c>
       <c r="G209" t="n">
-        <v>9.114579597119153</v>
+        <v>6146.401717724654</v>
       </c>
       <c r="H209" t="n">
         <v>4.382672594590874</v>
@@ -7682,7 +7682,7 @@
         </is>
       </c>
       <c r="G210" t="n">
-        <v>10.2424940561882</v>
+        <v>8341.141605321754</v>
       </c>
       <c r="H210" t="n">
         <v>4.788063036075911</v>
@@ -7718,7 +7718,7 @@
         </is>
       </c>
       <c r="G211" t="n">
-        <v>23.98160811264387</v>
+        <v>16853.46557951315</v>
       </c>
       <c r="H211" t="n">
         <v>2.226143426542681</v>
@@ -7752,7 +7752,7 @@
         <v>46</v>
       </c>
       <c r="G212" t="n">
-        <v>5.445641944318584</v>
+        <v>5179.15389591168</v>
       </c>
       <c r="H212" t="n">
         <v>5.885877676113296</v>
@@ -7788,7 +7788,7 @@
         </is>
       </c>
       <c r="G213" t="n">
-        <v>8.958358895611021</v>
+        <v>5787.952651914711</v>
       </c>
       <c r="H213" t="n">
         <v>4.972503428049746</v>
@@ -7822,7 +7822,7 @@
         </is>
       </c>
       <c r="G214" t="n">
-        <v>8.166705768369848</v>
+        <v>5311.576396227605</v>
       </c>
       <c r="H214" t="n">
         <v>7.701016901095828</v>
@@ -7858,7 +7858,7 @@
         </is>
       </c>
       <c r="G215" t="n">
-        <v>13.27234499251299</v>
+        <v>9076.35172738652</v>
       </c>
       <c r="H215" t="n">
         <v>7.701016901095828</v>
@@ -7894,7 +7894,7 @@
         </is>
       </c>
       <c r="G216" t="n">
-        <v>10.45882398246637</v>
+        <v>8615.672701122623</v>
       </c>
       <c r="H216" t="n">
         <v>8.305513683434167</v>
@@ -7928,7 +7928,7 @@
         <v>89</v>
       </c>
       <c r="G217" t="n">
-        <v>6.102663734500047</v>
+        <v>12487.60692726359</v>
       </c>
       <c r="H217" t="n">
         <v>10.9446445864214</v>
@@ -7962,7 +7962,7 @@
         <v>241</v>
       </c>
       <c r="G218" t="n">
-        <v>7.096813261690588</v>
+        <v>280274.7046598364</v>
       </c>
       <c r="H218" t="n">
         <v>8.177549813346189</v>
@@ -7998,7 +7998,7 @@
         </is>
       </c>
       <c r="G219" t="n">
-        <v>19.25714861232652</v>
+        <v>87737.01008189516</v>
       </c>
       <c r="H219" t="n">
         <v>15.36668796920312</v>
@@ -8032,7 +8032,7 @@
         <v>193</v>
       </c>
       <c r="G220" t="n">
-        <v>6.874999622242146</v>
+        <v>104934.7341706735</v>
       </c>
       <c r="H220" t="n">
         <v>16.8657746620857</v>
@@ -8066,7 +8066,7 @@
         <v>126.5</v>
       </c>
       <c r="G221" t="n">
-        <v>6.45332495388369</v>
+        <v>26903.63532694483</v>
       </c>
       <c r="H221" t="n">
         <v>6.640595692743264</v>
@@ -8100,7 +8100,7 @@
         <v>119.3</v>
       </c>
       <c r="G222" t="n">
-        <v>6.394859346939485</v>
+        <v>23217.27642042495</v>
       </c>
       <c r="H222" t="n">
         <v>6.544939925643833</v>
@@ -8134,7 +8134,7 @@
         <v>76.59999999999999</v>
       </c>
       <c r="G223" t="n">
-        <v>5.953139952320676</v>
+        <v>9688.521828905703</v>
       </c>
       <c r="H223" t="n">
         <v>6.500662841968202</v>
@@ -8168,7 +8168,7 @@
         <v>99.7</v>
       </c>
       <c r="G224" t="n">
-        <v>6.215851125543776</v>
+        <v>15544.96965563676</v>
       </c>
       <c r="H224" t="n">
         <v>5.890922190579032</v>
@@ -8202,7 +8202,7 @@
         <v>94.40000000000001</v>
       </c>
       <c r="G225" t="n">
-        <v>6.161386208647438</v>
+        <v>13946.94189672407</v>
       </c>
       <c r="H225" t="n">
         <v>9.503248678973984</v>
@@ -8236,7 +8236,7 @@
         <v>84.3</v>
       </c>
       <c r="G226" t="n">
-        <v>6.048586807516625</v>
+        <v>11342.31334280282</v>
       </c>
       <c r="H226" t="n">
         <v>6.10517149468766</v>
@@ -8270,7 +8270,7 @@
         <v>74.90000000000001</v>
       </c>
       <c r="G227" t="n">
-        <v>5.930780720413973</v>
+        <v>9357.212296618602</v>
       </c>
       <c r="H227" t="n">
         <v>6.368136669271553</v>
@@ -8304,7 +8304,7 @@
         <v>49</v>
       </c>
       <c r="G228" t="n">
-        <v>5.508444571583759</v>
+        <v>5507.130347478886</v>
       </c>
       <c r="H228" t="n">
         <v>7.001348300925303</v>
@@ -8338,7 +8338,7 @@
         <v>116</v>
       </c>
       <c r="G229" t="n">
-        <v>6.366875863821015</v>
+        <v>21700.91661735723</v>
       </c>
       <c r="H229" t="n">
         <v>11.64667333084614</v>
@@ -8374,7 +8374,7 @@
         </is>
       </c>
       <c r="G230" t="n">
-        <v>12.71647813637569</v>
+        <v>42522.54283539106</v>
       </c>
       <c r="H230" t="n">
         <v>8.940948848051857</v>
@@ -8408,7 +8408,7 @@
         </is>
       </c>
       <c r="G231" t="n">
-        <v>20.18298220606456</v>
+        <v>16009.42775520738</v>
       </c>
       <c r="H231" t="n">
         <v>5.349839111514215</v>
@@ -8442,7 +8442,7 @@
         <v>125</v>
       </c>
       <c r="G232" t="n">
-        <v>6.441423300967839</v>
+        <v>26090.2173846496</v>
       </c>
       <c r="H232" t="n">
         <v>10.65027234094756</v>
@@ -8476,7 +8476,7 @@
         <v>102</v>
       </c>
       <c r="G233" t="n">
-        <v>6.238594119972486</v>
+        <v>16294.24438990793</v>
       </c>
       <c r="H233" t="n">
         <v>14.39937412238358</v>
@@ -8510,7 +8510,7 @@
         <v>121</v>
       </c>
       <c r="G234" t="n">
-        <v>6.408975149416898</v>
+        <v>24039.32734200243</v>
       </c>
       <c r="H234" t="n">
         <v>14.54624402067073</v>
@@ -8544,7 +8544,7 @@
         <v>189</v>
       </c>
       <c r="G235" t="n">
-        <v>6.854087588999717</v>
+        <v>96686.06386388336</v>
       </c>
       <c r="H235" t="n">
         <v>13.13306229526616</v>
@@ -8580,7 +8580,7 @@
         </is>
       </c>
       <c r="G236" t="n">
-        <v>11.55841777930099</v>
+        <v>17520.86642387672</v>
       </c>
       <c r="H236" t="n">
         <v>11.22004124629944</v>
@@ -8614,7 +8614,7 @@
         <v>186</v>
       </c>
       <c r="G237" t="n">
-        <v>6.838111481403041</v>
+        <v>90927.93755467159</v>
       </c>
       <c r="H237" t="n">
         <v>17.06025824409521</v>
@@ -8650,7 +8650,7 @@
         </is>
       </c>
       <c r="G238" t="n">
-        <v>12.41728778045673</v>
+        <v>35737.96803215872</v>
       </c>
       <c r="H238" t="n">
         <v>16.67200337294842</v>
@@ -8684,7 +8684,7 @@
         <v>95</v>
       </c>
       <c r="G239" t="n">
-        <v>6.167703056293158</v>
+        <v>14119.27183211155</v>
       </c>
       <c r="H239" t="n">
         <v>16.8657746620857</v>
@@ -8718,7 +8718,7 @@
         <v>208</v>
       </c>
       <c r="G240" t="n">
-        <v>6.949741395649196</v>
+        <v>142643.4931878904</v>
       </c>
       <c r="H240" t="n">
         <v>16.67200337294842</v>
@@ -8752,7 +8752,7 @@
         <v>287</v>
       </c>
       <c r="G241" t="n">
-        <v>7.271309605612142</v>
+        <v>718572.921479625</v>
       </c>
       <c r="H241" t="n">
         <v>28.18833068636442</v>
@@ -8786,7 +8786,7 @@
         <v>57</v>
       </c>
       <c r="G242" t="n">
-        <v>5.658865300768017</v>
+        <v>6486.883952754216</v>
       </c>
       <c r="H242" t="inlineStr"/>
       <c r="I242" t="n">
@@ -8818,7 +8818,7 @@
         <v>42</v>
       </c>
       <c r="G243" t="n">
-        <v>5.355255200506476</v>
+        <v>4772.032905010629</v>
       </c>
       <c r="H243" t="inlineStr"/>
       <c r="I243" t="n">
@@ -8850,7 +8850,7 @@
         <v>64.5</v>
       </c>
       <c r="G244" t="n">
-        <v>5.781901795344783</v>
+        <v>7563.145896277892</v>
       </c>
       <c r="H244" t="inlineStr"/>
       <c r="I244" t="n">
@@ -8882,7 +8882,7 @@
         <v>53</v>
       </c>
       <c r="G245" t="n">
-        <v>5.586480573236176</v>
+        <v>5976.965407026083</v>
       </c>
       <c r="H245" t="inlineStr"/>
       <c r="I245" t="n">
@@ -8914,7 +8914,7 @@
         <v>54</v>
       </c>
       <c r="G246" t="n">
-        <v>5.6050738600417</v>
+        <v>6100.558399096927</v>
       </c>
       <c r="H246" t="inlineStr"/>
       <c r="I246" t="n">
@@ -8946,7 +8946,7 @@
         <v>47</v>
       </c>
       <c r="G247" t="n">
-        <v>5.467017403580413</v>
+        <v>5286.249567845563</v>
       </c>
       <c r="H247" t="inlineStr"/>
       <c r="I247" t="n">
@@ -8978,7 +8978,7 @@
         <v>77</v>
       </c>
       <c r="G248" t="n">
-        <v>5.958329081223977</v>
+        <v>9768.166660048983</v>
       </c>
       <c r="H248" t="inlineStr"/>
       <c r="I248" t="n">
@@ -9038,7 +9038,7 @@
         <v>157.5</v>
       </c>
       <c r="G250" t="n">
-        <v>6.672066489202267</v>
+        <v>50741.72324599716</v>
       </c>
       <c r="H250" t="inlineStr"/>
       <c r="I250" t="n">
@@ -9072,7 +9072,7 @@
         </is>
       </c>
       <c r="G251" t="n">
-        <v>26.81940399008904</v>
+        <v>24635.65156654295</v>
       </c>
       <c r="H251" t="inlineStr"/>
       <c r="I251" t="n">
@@ -9104,7 +9104,7 @@
         <v>36.5</v>
       </c>
       <c r="G252" t="n">
-        <v>5.215910825553951</v>
+        <v>4263.976213484621</v>
       </c>
       <c r="H252" t="n">
         <v>6.255766747657922</v>
@@ -9136,7 +9136,7 @@
         <v>102</v>
       </c>
       <c r="G253" t="n">
-        <v>6.238594119972486</v>
+        <v>16294.24438990793</v>
       </c>
       <c r="H253" t="inlineStr"/>
       <c r="I253" t="inlineStr"/>
@@ -9168,7 +9168,7 @@
         </is>
       </c>
       <c r="G254" t="n">
-        <v>14.67395126196438</v>
+        <v>10606.70497207723</v>
       </c>
       <c r="H254" t="inlineStr"/>
       <c r="I254" t="n">
@@ -9200,7 +9200,7 @@
         <v>93</v>
       </c>
       <c r="G255" t="n">
-        <v>6.146489844345901</v>
+        <v>13552.97403755158</v>
       </c>
       <c r="H255" t="inlineStr"/>
       <c r="I255" t="n">
@@ -9232,7 +9232,7 @@
         <v>88</v>
       </c>
       <c r="G256" t="n">
-        <v>6.091400375720581</v>
+        <v>12234.61685603116</v>
       </c>
       <c r="H256" t="inlineStr"/>
       <c r="I256" t="n">
@@ -9264,7 +9264,7 @@
         <v>75</v>
       </c>
       <c r="G257" t="n">
-        <v>5.932109899782458</v>
+        <v>9376.383620367058</v>
       </c>
       <c r="H257" t="inlineStr"/>
       <c r="I257" t="n">

</xml_diff>